<commit_message>
Upload Statement route complete
</commit_message>
<xml_diff>
--- a/DateFormats.xlsx
+++ b/DateFormats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://infosystechnologies-my.sharepoint.com/personal/amritanshu_ad_infosys_com/Documents/VB code/Python Code/Bank Statement Analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E865F950-1E02-4286-9C01-E3BE1A158347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{E865F950-1E02-4286-9C01-E3BE1A158347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{601D8F3A-1850-4EA0-8BC5-5A2D575DC51F}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5A3515E7-D34F-4BF2-A838-ACB3AB60ABD7}"/>
   </bookViews>
@@ -16,6 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$39</definedName>
     <definedName name="kanchor923" localSheetId="0">Sheet1!#REF!</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="113">
   <si>
     <t>MM/DD/YY</t>
   </si>
@@ -232,13 +233,157 @@
   </si>
   <si>
     <t>py_date</t>
+  </si>
+  <si>
+    <t>%m/%d/%Y</t>
+  </si>
+  <si>
+    <t>mm/dd/yyyy</t>
+  </si>
+  <si>
+    <t>%d/%m/%Y</t>
+  </si>
+  <si>
+    <t>dd/mm/yyyy</t>
+  </si>
+  <si>
+    <t>21/02/2018</t>
+  </si>
+  <si>
+    <t>%d/%m/%y</t>
+  </si>
+  <si>
+    <t>dd/mm/yy</t>
+  </si>
+  <si>
+    <t>21/02/18</t>
+  </si>
+  <si>
+    <t>%d-%m-%Y</t>
+  </si>
+  <si>
+    <t>dd-mm-yyyy</t>
+  </si>
+  <si>
+    <t>21-02-2018</t>
+  </si>
+  <si>
+    <t>%d-%m-%y</t>
+  </si>
+  <si>
+    <t>dd-mm-yy</t>
+  </si>
+  <si>
+    <t>21-02-18</t>
+  </si>
+  <si>
+    <t>%m-%d-%Y</t>
+  </si>
+  <si>
+    <t>mm-dd-yyyy</t>
+  </si>
+  <si>
+    <t>%m-%d-%y</t>
+  </si>
+  <si>
+    <t>mm-dd-yy</t>
+  </si>
+  <si>
+    <t>%Y-%m-%d</t>
+  </si>
+  <si>
+    <t>yyyy-mm-dd</t>
+  </si>
+  <si>
+    <t>m/d/yyyy</t>
+  </si>
+  <si>
+    <t>d/m/yyyy</t>
+  </si>
+  <si>
+    <t>21/2/2018</t>
+  </si>
+  <si>
+    <t>m-d-yyyy</t>
+  </si>
+  <si>
+    <t>m-d-yy</t>
+  </si>
+  <si>
+    <t>d-m-yyyy</t>
+  </si>
+  <si>
+    <t>21-2-2018</t>
+  </si>
+  <si>
+    <t>d-m-yy</t>
+  </si>
+  <si>
+    <t>21-2-18</t>
+  </si>
+  <si>
+    <t>Mth d, yyyy</t>
+  </si>
+  <si>
+    <t>Month d, yyyy</t>
+  </si>
+  <si>
+    <t>%B %d, %Y</t>
+  </si>
+  <si>
+    <t>%-m/%-d/%Y</t>
+  </si>
+  <si>
+    <t>%-d/%-m/%Y</t>
+  </si>
+  <si>
+    <t>%-m-%-d-%Y</t>
+  </si>
+  <si>
+    <t>%-m-%-d-%y</t>
+  </si>
+  <si>
+    <t>%-d-%-m-%Y</t>
+  </si>
+  <si>
+    <t>%-d-%-m-%y</t>
+  </si>
+  <si>
+    <t>%b %-d, %Y</t>
+  </si>
+  <si>
+    <t>%Y-%b-%d</t>
+  </si>
+  <si>
+    <t>02/21/2018</t>
+  </si>
+  <si>
+    <t>02-21-18</t>
+  </si>
+  <si>
+    <t>2018-02-21</t>
+  </si>
+  <si>
+    <t>2/21/2018</t>
+  </si>
+  <si>
+    <t>2-21-2018</t>
+  </si>
+  <si>
+    <t>2-21-18</t>
+  </si>
+  <si>
+    <t>Feb 21, 2018</t>
+  </si>
+  <si>
+    <t>February 21, 2018</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -259,8 +404,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF525252"/>
+      <name val="Inherit"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -279,8 +429,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF4F4F4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -303,11 +459,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FFF4F4F4"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFE0E0E0"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -318,11 +485,28 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -632,19 +816,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{790DDE7D-4A9F-4ACB-9EBB-4DC621CCC996}">
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="2" width="38.42578125" customWidth="1"/>
     <col min="3" max="3" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="26.25" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>62</v>
       </c>
@@ -655,7 +837,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="25.5">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -666,7 +848,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="25.5">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -677,7 +859,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="25.5">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
@@ -688,7 +870,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="25.5">
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
@@ -699,7 +881,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="25.5">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -710,7 +892,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="25.5">
       <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
@@ -721,7 +903,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="25.5">
       <c r="A8" s="3" t="s">
         <v>12</v>
       </c>
@@ -732,7 +914,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="25.5">
       <c r="A9" s="2" t="s">
         <v>14</v>
       </c>
@@ -743,7 +925,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="25.5">
       <c r="A10" s="3" t="s">
         <v>16</v>
       </c>
@@ -754,7 +936,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="25.5">
       <c r="A11" s="2" t="s">
         <v>18</v>
       </c>
@@ -765,7 +947,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="25.5">
       <c r="A12" s="3" t="s">
         <v>20</v>
       </c>
@@ -776,7 +958,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="25.5">
       <c r="A13" s="2" t="s">
         <v>22</v>
       </c>
@@ -787,7 +969,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="25.5">
       <c r="A14" s="3" t="s">
         <v>24</v>
       </c>
@@ -798,7 +980,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3">
       <c r="A15" s="2" t="s">
         <v>26</v>
       </c>
@@ -809,7 +991,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3">
       <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
@@ -820,7 +1002,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="25.5">
       <c r="A17" s="2" t="s">
         <v>30</v>
       </c>
@@ -831,7 +1013,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="25.5">
       <c r="A18" s="3" t="s">
         <v>32</v>
       </c>
@@ -842,7 +1024,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="25.5">
       <c r="A19" s="2" t="s">
         <v>33</v>
       </c>
@@ -850,10 +1032,10 @@
         <v>42</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="25.5">
       <c r="A20" s="3" t="s">
         <v>34</v>
       </c>
@@ -864,7 +1046,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="25.5">
       <c r="A21" s="2" t="s">
         <v>35</v>
       </c>
@@ -875,7 +1057,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" ht="26.25" thickBot="1">
       <c r="A22" s="3" t="s">
         <v>36</v>
       </c>
@@ -886,7 +1068,195 @@
         <v>59</v>
       </c>
     </row>
+    <row r="23" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A23" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A24" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A25" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A26" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A27" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A28" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A29" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A30" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A31" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A32" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A33" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A34" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A35" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="C35" s="4" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A36" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A37" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A38" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" ht="15.75" thickBot="1">
+      <c r="A39" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>96</v>
+      </c>
+    </row>
   </sheetData>
+  <autoFilter ref="A1:C39" xr:uid="{790DDE7D-4A9F-4ACB-9EBB-4DC621CCC996}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
 </worksheet>

</xml_diff>